<commit_message>
Initial Data File Updated
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF44EC56-CAE6-48A5-ACAA-4A3D25123854}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A094C92A-D8E3-437E-85B0-CB5761BC4805}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>Proyección Post-Quincena</t>
+  </si>
+  <si>
+    <t>Ingreso de monedas a alcancía</t>
+  </si>
+  <si>
+    <t>ahorro</t>
+  </si>
+  <si>
+    <t>Alcancía</t>
   </si>
 </sst>
 </file>
@@ -233,9 +242,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -525,7 +535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V16" sqref="V16"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,21 +550,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -629,11 +639,11 @@
         <v>170</v>
       </c>
       <c r="N4" s="2">
-        <f>SUM(K4:M4)</f>
+        <f t="shared" ref="N4:N10" si="0">SUM(K4:M4)</f>
         <v>9737.82</v>
       </c>
       <c r="O4" s="2">
-        <f>N4-4000</f>
+        <f t="shared" ref="O4:O11" si="1">N4-4000</f>
         <v>5737.82</v>
       </c>
     </row>
@@ -670,11 +680,11 @@
         <v>170</v>
       </c>
       <c r="N5">
-        <f>SUM(K5:M5)</f>
+        <f t="shared" si="0"/>
         <v>11845.82</v>
       </c>
       <c r="O5">
-        <f>N5-4000</f>
+        <f t="shared" si="1"/>
         <v>7845.82</v>
       </c>
     </row>
@@ -712,11 +722,11 @@
         <v>3370</v>
       </c>
       <c r="N6" s="2">
-        <f>SUM(K6:M6)</f>
+        <f t="shared" si="0"/>
         <v>11845.82</v>
       </c>
       <c r="O6" s="2">
-        <f>N6-4000</f>
+        <f t="shared" si="1"/>
         <v>7845.82</v>
       </c>
     </row>
@@ -753,11 +763,11 @@
         <v>120</v>
       </c>
       <c r="N7" s="2">
-        <f>SUM(K7:M7)</f>
+        <f t="shared" si="0"/>
         <v>8595.82</v>
       </c>
       <c r="O7" s="2">
-        <f>N7-4000</f>
+        <f t="shared" si="1"/>
         <v>4595.82</v>
       </c>
     </row>
@@ -795,11 +805,11 @@
         <v>120</v>
       </c>
       <c r="N8" s="2">
-        <f>SUM(K8:M8)</f>
+        <f t="shared" si="0"/>
         <v>8595.82</v>
       </c>
       <c r="O8" s="2">
-        <f>N8-4000</f>
+        <f t="shared" si="1"/>
         <v>4595.82</v>
       </c>
     </row>
@@ -836,11 +846,11 @@
         <v>95</v>
       </c>
       <c r="N9" s="2">
-        <f>SUM(K9:M9)</f>
+        <f t="shared" si="0"/>
         <v>8570.82</v>
       </c>
       <c r="O9" s="2">
-        <f>N9-4000</f>
+        <f t="shared" si="1"/>
         <v>4570.82</v>
       </c>
     </row>
@@ -877,16 +887,54 @@
         <v>95</v>
       </c>
       <c r="N10" s="2">
-        <f>SUM(K10:M10)</f>
+        <f t="shared" si="0"/>
         <v>8501.82</v>
       </c>
       <c r="O10" s="2">
-        <f>N10-4000</f>
+        <f t="shared" si="1"/>
         <v>4501.82</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>43526</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>8256.82</v>
+      </c>
+      <c r="L11">
+        <v>150</v>
+      </c>
+      <c r="M11">
+        <f>M10-B11</f>
+        <v>90</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" ref="N11" si="2">SUM(K11:M11)</f>
+        <v>8496.82</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="1"/>
+        <v>4496.82</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
Initial Data File Updated, Debt table and calculations added
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D3385-0AD7-4DFD-AE1A-3C358709A44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1AF0A9-58E5-4803-9FD4-5E513DCA2A91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Transacciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Deudas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -212,6 +213,57 @@
   </si>
   <si>
     <t>Propina Buffete de Carnes</t>
+  </si>
+  <si>
+    <t>Renta 1er departamento</t>
+  </si>
+  <si>
+    <t>Depósito 1er departamento</t>
+  </si>
+  <si>
+    <t>1er Mes de Manutención</t>
+  </si>
+  <si>
+    <t>Renta 2do Departamento</t>
+  </si>
+  <si>
+    <t>Depósito 2do Departamento</t>
+  </si>
+  <si>
+    <t>Xbox One X</t>
+  </si>
+  <si>
+    <t>iPhone 8 Plus</t>
+  </si>
+  <si>
+    <t>Deuda Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monto </t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Deuda Rentas</t>
+  </si>
+  <si>
+    <t>Deuda Restante (Rentas)</t>
+  </si>
+  <si>
+    <t>Deuda Restante (Total)</t>
+  </si>
+  <si>
+    <t>TV Sharp 4K 50"</t>
+  </si>
+  <si>
+    <t>Estimado Meses restantes</t>
+  </si>
+  <si>
+    <t>Pago mensual</t>
+  </si>
+  <si>
+    <t>Pago de Recibo de Electricidad</t>
   </si>
 </sst>
 </file>
@@ -260,9 +312,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -552,9 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,21 +622,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -751,7 +804,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43525</v>
+        <v>43556</v>
       </c>
       <c r="B7">
         <v>3250</v>
@@ -792,7 +845,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43525</v>
+        <v>43556</v>
       </c>
       <c r="B8" s="2">
         <v>1599.46</v>
@@ -834,7 +887,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43526</v>
+        <v>43557</v>
       </c>
       <c r="B9" s="2">
         <v>25</v>
@@ -875,7 +928,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43526</v>
+        <v>43557</v>
       </c>
       <c r="B10" s="2">
         <v>69</v>
@@ -916,7 +969,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43526</v>
+        <v>43557</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -963,7 +1016,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43527</v>
+        <v>43558</v>
       </c>
       <c r="B12">
         <v>225</v>
@@ -1014,7 +1067,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43527</v>
+        <v>43558</v>
       </c>
       <c r="B13">
         <v>200</v>
@@ -1055,7 +1108,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43527</v>
+        <v>43558</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -1107,19 +1160,58 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43559</v>
+      </c>
+      <c r="B15">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>7831.82</v>
+      </c>
+      <c r="L15">
+        <f>L14-B15</f>
+        <v>87</v>
+      </c>
+      <c r="M15">
+        <v>70</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" ref="N15" si="9">SUM(K15:M15)</f>
+        <v>7988.82</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" ref="O15" si="10">N15-4000</f>
+        <v>3988.8199999999997</v>
+      </c>
       <c r="S15">
-        <v>4501.82</v>
+        <v>3988.82</v>
       </c>
       <c r="T15">
         <v>250</v>
       </c>
       <c r="U15">
         <f>S15-T19</f>
-        <v>3551.8199999999997</v>
+        <v>3188.82</v>
       </c>
       <c r="V15">
         <f>U15+U12</f>
-        <v>7877.82</v>
+        <v>7514.82</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1129,7 +1221,7 @@
     </row>
     <row r="17" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T17">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="20:20" x14ac:dyDescent="0.25">
@@ -1140,7 +1232,7 @@
     <row r="19" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T19">
         <f>SUM(T15:T18)</f>
-        <v>950</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -1151,4 +1243,210 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D27017-4FBF-41C0-A2E3-E97A51044A46}">
+  <dimension ref="A2:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2">
+        <f>SUM($B4:$B8)</f>
+        <v>15900</v>
+      </c>
+      <c r="M2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2">
+        <f>IF((G2-SUM(J:J)) &lt;= 0,0,G2-SUM(J:J))</f>
+        <v>1000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3">
+        <f>SUM(B:B)</f>
+        <v>58483</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3">
+        <f>G3-SUM(J:J)</f>
+        <v>43583</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3">
+        <f>N3/Q2</f>
+        <v>14.527666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2500</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="1">
+        <v>43422</v>
+      </c>
+      <c r="J4">
+        <v>2400</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2500</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="1">
+        <v>43449</v>
+      </c>
+      <c r="J5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="1">
+        <v>43462</v>
+      </c>
+      <c r="J6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4900</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="1">
+        <v>43480</v>
+      </c>
+      <c r="J7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="1">
+        <v>43496</v>
+      </c>
+      <c r="J8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>11759</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="1">
+        <v>43511</v>
+      </c>
+      <c r="J9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>20324</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="1">
+        <v>43524</v>
+      </c>
+      <c r="J10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10500</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="1">
+        <v>43539</v>
+      </c>
+      <c r="J11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>43553</v>
+      </c>
+      <c r="J12">
+        <v>1500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial Data File Update
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2628D9A0-4A59-43C9-943A-D78318FE9F98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8303950-97F6-4C80-8E76-CC85CDDE0121}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="101">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>Garrafón Ciel</t>
+  </si>
+  <si>
+    <t>Licuado</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -466,6 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -750,11 +754,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,21 +773,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2151,6 +2155,88 @@
       <c r="O34">
         <f t="shared" si="27"/>
         <v>3923.6400000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43567</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>81</v>
+      </c>
+      <c r="K35">
+        <v>7358.64</v>
+      </c>
+      <c r="L35">
+        <f>L34-B35</f>
+        <v>46</v>
+      </c>
+      <c r="M35">
+        <v>504</v>
+      </c>
+      <c r="N35" s="14">
+        <f t="shared" ref="N35" si="28">SUM(K35:M35)</f>
+        <v>7908.64</v>
+      </c>
+      <c r="O35" s="14">
+        <f t="shared" ref="O35" si="29">N35-4000</f>
+        <v>3908.6400000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43567</v>
+      </c>
+      <c r="B36">
+        <v>13.5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36">
+        <v>7358.64</v>
+      </c>
+      <c r="L36">
+        <f>L35-B36</f>
+        <v>32.5</v>
+      </c>
+      <c r="M36">
+        <v>504</v>
+      </c>
+      <c r="N36" s="14">
+        <f t="shared" ref="N36" si="30">SUM(K36:M36)</f>
+        <v>7895.14</v>
+      </c>
+      <c r="O36" s="14">
+        <f t="shared" ref="O36" si="31">N36-4000</f>
+        <v>3895.1400000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2440,15 +2526,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Intial Data File Updated
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EA56A2-25FB-443B-8C12-5B52E4841796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B397696-BC45-42C7-87BC-7DD5D91FAB33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="169">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>Axtel</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galletas </t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -722,6 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1010,11 +1017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V93"/>
+  <dimension ref="A1:V96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P93" sqref="P93"/>
+      <pane ySplit="3" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R96" sqref="R96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,21 +1037,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4905,6 +4912,141 @@
       <c r="P93" s="27">
         <f>O93-Ahorros!$E$4</f>
         <v>570.01000000000022</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>43579</v>
+      </c>
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>125</v>
+      </c>
+      <c r="D94" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" t="s">
+        <v>22</v>
+      </c>
+      <c r="F94" t="s">
+        <v>32</v>
+      </c>
+      <c r="G94" t="s">
+        <v>81</v>
+      </c>
+      <c r="K94">
+        <f>K93-B94</f>
+        <v>6756.44</v>
+      </c>
+      <c r="L94">
+        <v>2298.5700000000002</v>
+      </c>
+      <c r="M94">
+        <v>2</v>
+      </c>
+      <c r="N94" s="31">
+        <f t="shared" ref="N94:N95" si="93">SUM(K94:M94)</f>
+        <v>9057.01</v>
+      </c>
+      <c r="O94" s="31">
+        <f t="shared" ref="O94:O95" si="94">N94-4000</f>
+        <v>5057.01</v>
+      </c>
+      <c r="P94" s="27">
+        <f>O94-Ahorros!$E$4</f>
+        <v>557.01000000000022</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>43580</v>
+      </c>
+      <c r="B95">
+        <v>200</v>
+      </c>
+      <c r="C95" t="s">
+        <v>167</v>
+      </c>
+      <c r="D95" t="s">
+        <v>48</v>
+      </c>
+      <c r="E95" t="s">
+        <v>22</v>
+      </c>
+      <c r="F95" t="s">
+        <v>32</v>
+      </c>
+      <c r="G95" t="s">
+        <v>81</v>
+      </c>
+      <c r="K95">
+        <f>K94-B95</f>
+        <v>6556.44</v>
+      </c>
+      <c r="L95">
+        <v>2298.5700000000002</v>
+      </c>
+      <c r="M95">
+        <v>2</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="93"/>
+        <v>8857.01</v>
+      </c>
+      <c r="O95">
+        <f t="shared" si="94"/>
+        <v>4857.01</v>
+      </c>
+      <c r="P95" s="27">
+        <f>O95-Ahorros!$E$4</f>
+        <v>357.01000000000022</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>43581</v>
+      </c>
+      <c r="B96">
+        <v>24</v>
+      </c>
+      <c r="C96" t="s">
+        <v>168</v>
+      </c>
+      <c r="D96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" t="s">
+        <v>22</v>
+      </c>
+      <c r="F96" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" t="s">
+        <v>81</v>
+      </c>
+      <c r="K96">
+        <v>6556.44</v>
+      </c>
+      <c r="L96">
+        <f>L95-B96</f>
+        <v>2274.5700000000002</v>
+      </c>
+      <c r="M96">
+        <v>2</v>
+      </c>
+      <c r="N96" s="31">
+        <f t="shared" ref="N96" si="95">SUM(K96:M96)</f>
+        <v>8833.01</v>
+      </c>
+      <c r="O96" s="31">
+        <f t="shared" ref="O96" si="96">N96-4000</f>
+        <v>4833.01</v>
+      </c>
+      <c r="P96" s="27">
+        <f>O96-Ahorros!$E$4</f>
+        <v>333.01000000000022</v>
       </c>
     </row>
   </sheetData>
@@ -5205,15 +5347,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Initial Data Fiel Update
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D06A9E-95CB-446C-9027-268FD8DE5308}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD86A45C-9CCA-403E-B3C1-096A927DA43B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="213">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -673,6 +673,33 @@
   </si>
   <si>
     <t>Ligerisimo</t>
+  </si>
+  <si>
+    <t>Atun</t>
+  </si>
+  <si>
+    <t>Barritas</t>
+  </si>
+  <si>
+    <t>Barritas de Pescado</t>
+  </si>
+  <si>
+    <t>Paketaxo</t>
+  </si>
+  <si>
+    <t>Chuleta de Cerdo</t>
+  </si>
+  <si>
+    <t>Ensalda de Vegetales</t>
+  </si>
+  <si>
+    <t>Jamón de Pavo</t>
+  </si>
+  <si>
+    <t>Frijoles la Sierra</t>
+  </si>
+  <si>
+    <t>Queso Chihuahua</t>
   </si>
 </sst>
 </file>
@@ -825,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -865,6 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1150,11 +1178,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V133"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
+      <pane ySplit="3" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R149" sqref="R149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,21 +1198,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5273,6 +5301,9 @@
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>43582</v>
+      </c>
       <c r="B99">
         <v>34</v>
       </c>
@@ -5360,6 +5391,9 @@
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>43583</v>
+      </c>
       <c r="B101">
         <v>200</v>
       </c>
@@ -5403,6 +5437,9 @@
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>43583</v>
+      </c>
       <c r="B102">
         <v>94</v>
       </c>
@@ -5445,6 +5482,9 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>43583</v>
+      </c>
       <c r="B103">
         <v>35</v>
       </c>
@@ -5487,6 +5527,9 @@
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>43583</v>
+      </c>
       <c r="B104">
         <v>5</v>
       </c>
@@ -5529,6 +5572,9 @@
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>43583</v>
+      </c>
       <c r="B105">
         <v>15</v>
       </c>
@@ -5616,6 +5662,9 @@
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>43583</v>
+      </c>
       <c r="B107">
         <v>34</v>
       </c>
@@ -5658,6 +5707,9 @@
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>43583</v>
+      </c>
       <c r="B108">
         <v>11.5</v>
       </c>
@@ -5700,6 +5752,9 @@
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>43583</v>
+      </c>
       <c r="B109">
         <v>13.5</v>
       </c>
@@ -5742,6 +5797,9 @@
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>43583</v>
+      </c>
       <c r="B110">
         <v>25.5</v>
       </c>
@@ -5784,6 +5842,9 @@
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>43583</v>
+      </c>
       <c r="B111">
         <v>21.5</v>
       </c>
@@ -5826,6 +5887,9 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>43583</v>
+      </c>
       <c r="B112">
         <v>14.95</v>
       </c>
@@ -5868,6 +5932,9 @@
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>43583</v>
+      </c>
       <c r="B113">
         <v>53.16</v>
       </c>
@@ -5910,6 +5977,9 @@
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>43583</v>
+      </c>
       <c r="B114">
         <v>37.25</v>
       </c>
@@ -5952,6 +6022,9 @@
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>43583</v>
+      </c>
       <c r="B115">
         <v>12</v>
       </c>
@@ -5994,6 +6067,9 @@
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>43583</v>
+      </c>
       <c r="B116">
         <v>23.5</v>
       </c>
@@ -6126,6 +6202,9 @@
       </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>43585</v>
+      </c>
       <c r="B119">
         <v>17</v>
       </c>
@@ -6168,6 +6247,9 @@
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>43585</v>
+      </c>
       <c r="B120">
         <v>6640</v>
       </c>
@@ -6210,6 +6292,9 @@
       </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>43585</v>
+      </c>
       <c r="B121">
         <v>15</v>
       </c>
@@ -6252,6 +6337,9 @@
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>43585</v>
+      </c>
       <c r="B122">
         <v>10</v>
       </c>
@@ -6339,6 +6427,9 @@
       </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>43586</v>
+      </c>
       <c r="B124">
         <v>5</v>
       </c>
@@ -6381,6 +6472,9 @@
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>43586</v>
+      </c>
       <c r="B125">
         <v>97.5</v>
       </c>
@@ -6423,6 +6517,9 @@
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>43586</v>
+      </c>
       <c r="B126">
         <v>3000</v>
       </c>
@@ -6465,6 +6562,9 @@
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>43586</v>
+      </c>
       <c r="B127">
         <v>13</v>
       </c>
@@ -6507,6 +6607,9 @@
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>43586</v>
+      </c>
       <c r="B128">
         <v>49</v>
       </c>
@@ -6598,6 +6701,9 @@
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>43587</v>
+      </c>
       <c r="B130">
         <v>200</v>
       </c>
@@ -6640,6 +6746,9 @@
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>43587</v>
+      </c>
       <c r="B131">
         <v>66</v>
       </c>
@@ -6682,6 +6791,9 @@
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>43587</v>
+      </c>
       <c r="B132">
         <v>53</v>
       </c>
@@ -6756,16 +6868,737 @@
         <v>69</v>
       </c>
       <c r="N133" s="36">
-        <f t="shared" ref="N133" si="137">SUM(K133:M133)</f>
+        <f t="shared" ref="N133:N134" si="137">SUM(K133:M133)</f>
         <v>9559.15</v>
       </c>
       <c r="O133" s="36">
-        <f t="shared" ref="O133" si="138">N133-4000</f>
+        <f t="shared" ref="O133:O134" si="138">N133-4000</f>
         <v>5559.15</v>
       </c>
       <c r="P133" s="25">
         <f>O133-Ahorros!$E$4</f>
         <v>559.14999999999964</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134" t="s">
+        <v>177</v>
+      </c>
+      <c r="D134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E134" t="s">
+        <v>22</v>
+      </c>
+      <c r="F134" t="s">
+        <v>7</v>
+      </c>
+      <c r="G134" t="s">
+        <v>44</v>
+      </c>
+      <c r="K134">
+        <v>5643.58</v>
+      </c>
+      <c r="L134">
+        <v>3846.57</v>
+      </c>
+      <c r="M134">
+        <f>M133-B134</f>
+        <v>59</v>
+      </c>
+      <c r="N134">
+        <f t="shared" si="137"/>
+        <v>9549.15</v>
+      </c>
+      <c r="O134">
+        <f t="shared" si="138"/>
+        <v>5549.15</v>
+      </c>
+      <c r="P134" s="25">
+        <f>O134-Ahorros!$E$4</f>
+        <v>549.14999999999964</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B135">
+        <v>19.55</v>
+      </c>
+      <c r="C135" t="s">
+        <v>204</v>
+      </c>
+      <c r="D135" t="s">
+        <v>82</v>
+      </c>
+      <c r="E135" t="s">
+        <v>22</v>
+      </c>
+      <c r="F135" t="s">
+        <v>18</v>
+      </c>
+      <c r="G135" t="s">
+        <v>84</v>
+      </c>
+      <c r="K135">
+        <f>5643.58</f>
+        <v>5643.58</v>
+      </c>
+      <c r="L135">
+        <f>L134-B135</f>
+        <v>3827.02</v>
+      </c>
+      <c r="M135">
+        <v>59</v>
+      </c>
+      <c r="N135" s="39">
+        <f t="shared" ref="N135" si="139">SUM(K135:M135)</f>
+        <v>9529.6</v>
+      </c>
+      <c r="O135" s="39">
+        <f t="shared" ref="O135" si="140">N135-4000</f>
+        <v>5529.6</v>
+      </c>
+      <c r="P135" s="25">
+        <f>O135-Ahorros!$E$4</f>
+        <v>529.60000000000036</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B136">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>205</v>
+      </c>
+      <c r="D136" t="s">
+        <v>69</v>
+      </c>
+      <c r="E136" t="s">
+        <v>22</v>
+      </c>
+      <c r="F136" t="s">
+        <v>18</v>
+      </c>
+      <c r="G136" t="s">
+        <v>84</v>
+      </c>
+      <c r="K136">
+        <v>5643.58</v>
+      </c>
+      <c r="L136">
+        <f>L135-B136</f>
+        <v>3802.02</v>
+      </c>
+      <c r="M136">
+        <v>59</v>
+      </c>
+      <c r="N136" s="39">
+        <f t="shared" ref="N136:N147" si="141">SUM(K136:M136)</f>
+        <v>9504.6</v>
+      </c>
+      <c r="O136" s="39">
+        <f t="shared" ref="O136:O147" si="142">N136-4000</f>
+        <v>5504.6</v>
+      </c>
+      <c r="P136" s="25">
+        <f>O136-Ahorros!$E$4</f>
+        <v>504.60000000000036</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B137">
+        <v>33.54</v>
+      </c>
+      <c r="C137" t="s">
+        <v>206</v>
+      </c>
+      <c r="D137" t="s">
+        <v>82</v>
+      </c>
+      <c r="E137" t="s">
+        <v>22</v>
+      </c>
+      <c r="F137" t="s">
+        <v>18</v>
+      </c>
+      <c r="G137" t="s">
+        <v>84</v>
+      </c>
+      <c r="K137">
+        <v>5643.58</v>
+      </c>
+      <c r="L137">
+        <f>L136-B137</f>
+        <v>3768.48</v>
+      </c>
+      <c r="M137">
+        <v>59</v>
+      </c>
+      <c r="N137">
+        <f t="shared" si="141"/>
+        <v>9471.06</v>
+      </c>
+      <c r="O137">
+        <f t="shared" si="142"/>
+        <v>5471.0599999999995</v>
+      </c>
+      <c r="P137" s="25">
+        <f>O137-Ahorros!$E$4</f>
+        <v>471.05999999999949</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B138">
+        <v>25</v>
+      </c>
+      <c r="C138" t="s">
+        <v>207</v>
+      </c>
+      <c r="D138" t="s">
+        <v>69</v>
+      </c>
+      <c r="E138" t="s">
+        <v>22</v>
+      </c>
+      <c r="F138" t="s">
+        <v>18</v>
+      </c>
+      <c r="G138" t="s">
+        <v>84</v>
+      </c>
+      <c r="K138">
+        <v>5643.58</v>
+      </c>
+      <c r="L138">
+        <f>L137-B138</f>
+        <v>3743.48</v>
+      </c>
+      <c r="M138">
+        <v>59</v>
+      </c>
+      <c r="N138">
+        <f t="shared" si="141"/>
+        <v>9446.06</v>
+      </c>
+      <c r="O138">
+        <f t="shared" si="142"/>
+        <v>5446.0599999999995</v>
+      </c>
+      <c r="P138" s="25">
+        <f>O138-Ahorros!$E$4</f>
+        <v>446.05999999999949</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B139">
+        <v>13.9</v>
+      </c>
+      <c r="C139" t="s">
+        <v>147</v>
+      </c>
+      <c r="D139" t="s">
+        <v>82</v>
+      </c>
+      <c r="E139" t="s">
+        <v>22</v>
+      </c>
+      <c r="F139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G139" t="s">
+        <v>84</v>
+      </c>
+      <c r="K139">
+        <v>5643.58</v>
+      </c>
+      <c r="L139">
+        <f>L138-B139</f>
+        <v>3729.58</v>
+      </c>
+      <c r="M139">
+        <v>59</v>
+      </c>
+      <c r="N139">
+        <f t="shared" si="141"/>
+        <v>9432.16</v>
+      </c>
+      <c r="O139">
+        <f t="shared" si="142"/>
+        <v>5432.16</v>
+      </c>
+      <c r="P139" s="25">
+        <f>O139-Ahorros!$E$4</f>
+        <v>432.15999999999985</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B140">
+        <v>35.33</v>
+      </c>
+      <c r="C140" t="s">
+        <v>208</v>
+      </c>
+      <c r="D140" t="s">
+        <v>82</v>
+      </c>
+      <c r="E140" t="s">
+        <v>22</v>
+      </c>
+      <c r="F140" t="s">
+        <v>18</v>
+      </c>
+      <c r="G140" t="s">
+        <v>84</v>
+      </c>
+      <c r="K140">
+        <v>5643.58</v>
+      </c>
+      <c r="L140">
+        <f>L139-B140</f>
+        <v>3694.25</v>
+      </c>
+      <c r="M140">
+        <v>59</v>
+      </c>
+      <c r="N140">
+        <f t="shared" si="141"/>
+        <v>9396.83</v>
+      </c>
+      <c r="O140">
+        <f t="shared" si="142"/>
+        <v>5396.83</v>
+      </c>
+      <c r="P140" s="25">
+        <f>O140-Ahorros!$E$4</f>
+        <v>396.82999999999993</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B141">
+        <v>11.5</v>
+      </c>
+      <c r="C141" t="s">
+        <v>125</v>
+      </c>
+      <c r="D141" t="s">
+        <v>69</v>
+      </c>
+      <c r="E141" t="s">
+        <v>22</v>
+      </c>
+      <c r="F141" t="s">
+        <v>18</v>
+      </c>
+      <c r="G141" t="s">
+        <v>84</v>
+      </c>
+      <c r="K141">
+        <v>5643.58</v>
+      </c>
+      <c r="L141">
+        <f>L140-B141</f>
+        <v>3682.75</v>
+      </c>
+      <c r="M141">
+        <v>59</v>
+      </c>
+      <c r="N141">
+        <f t="shared" si="141"/>
+        <v>9385.33</v>
+      </c>
+      <c r="O141">
+        <f t="shared" si="142"/>
+        <v>5385.33</v>
+      </c>
+      <c r="P141" s="25">
+        <f>O141-Ahorros!$E$4</f>
+        <v>385.32999999999993</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B142">
+        <v>13.5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>209</v>
+      </c>
+      <c r="D142" t="s">
+        <v>82</v>
+      </c>
+      <c r="E142" t="s">
+        <v>22</v>
+      </c>
+      <c r="F142" t="s">
+        <v>18</v>
+      </c>
+      <c r="G142" t="s">
+        <v>84</v>
+      </c>
+      <c r="K142">
+        <v>5643.58</v>
+      </c>
+      <c r="L142">
+        <f>L141-B142</f>
+        <v>3669.25</v>
+      </c>
+      <c r="M142">
+        <v>59</v>
+      </c>
+      <c r="N142">
+        <f t="shared" si="141"/>
+        <v>9371.83</v>
+      </c>
+      <c r="O142">
+        <f t="shared" si="142"/>
+        <v>5371.83</v>
+      </c>
+      <c r="P142" s="25">
+        <f>O142-Ahorros!$E$4</f>
+        <v>371.82999999999993</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B143">
+        <v>29.5</v>
+      </c>
+      <c r="C143" t="s">
+        <v>210</v>
+      </c>
+      <c r="D143" t="s">
+        <v>82</v>
+      </c>
+      <c r="E143" t="s">
+        <v>22</v>
+      </c>
+      <c r="F143" t="s">
+        <v>18</v>
+      </c>
+      <c r="G143" t="s">
+        <v>84</v>
+      </c>
+      <c r="K143">
+        <v>5643.58</v>
+      </c>
+      <c r="L143">
+        <f>L142-B143</f>
+        <v>3639.75</v>
+      </c>
+      <c r="M143">
+        <v>59</v>
+      </c>
+      <c r="N143">
+        <f t="shared" si="141"/>
+        <v>9342.33</v>
+      </c>
+      <c r="O143">
+        <f t="shared" si="142"/>
+        <v>5342.33</v>
+      </c>
+      <c r="P143" s="25">
+        <f>O143-Ahorros!$E$4</f>
+        <v>342.32999999999993</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B144">
+        <v>11.05</v>
+      </c>
+      <c r="C144" t="s">
+        <v>211</v>
+      </c>
+      <c r="D144" t="s">
+        <v>82</v>
+      </c>
+      <c r="E144" t="s">
+        <v>22</v>
+      </c>
+      <c r="F144" t="s">
+        <v>18</v>
+      </c>
+      <c r="G144" t="s">
+        <v>84</v>
+      </c>
+      <c r="K144">
+        <v>5643.58</v>
+      </c>
+      <c r="L144">
+        <f>L143-B144</f>
+        <v>3628.7</v>
+      </c>
+      <c r="M144">
+        <v>59</v>
+      </c>
+      <c r="N144">
+        <f t="shared" si="141"/>
+        <v>9331.2799999999988</v>
+      </c>
+      <c r="O144">
+        <f t="shared" si="142"/>
+        <v>5331.2799999999988</v>
+      </c>
+      <c r="P144" s="25">
+        <f>O144-Ahorros!$E$4</f>
+        <v>331.27999999999884</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B145">
+        <v>21.5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>183</v>
+      </c>
+      <c r="D145" t="s">
+        <v>82</v>
+      </c>
+      <c r="E145" t="s">
+        <v>22</v>
+      </c>
+      <c r="F145" t="s">
+        <v>18</v>
+      </c>
+      <c r="G145" t="s">
+        <v>84</v>
+      </c>
+      <c r="K145">
+        <v>5643.58</v>
+      </c>
+      <c r="L145">
+        <f>L144-B145</f>
+        <v>3607.2</v>
+      </c>
+      <c r="M145">
+        <v>59</v>
+      </c>
+      <c r="N145">
+        <f t="shared" si="141"/>
+        <v>9309.7799999999988</v>
+      </c>
+      <c r="O145">
+        <f t="shared" si="142"/>
+        <v>5309.7799999999988</v>
+      </c>
+      <c r="P145" s="25">
+        <f>O145-Ahorros!$E$4</f>
+        <v>309.77999999999884</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B146">
+        <v>37.25</v>
+      </c>
+      <c r="C146" t="s">
+        <v>87</v>
+      </c>
+      <c r="D146" t="s">
+        <v>82</v>
+      </c>
+      <c r="E146" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" t="s">
+        <v>18</v>
+      </c>
+      <c r="G146" t="s">
+        <v>84</v>
+      </c>
+      <c r="K146">
+        <v>5643.58</v>
+      </c>
+      <c r="L146">
+        <f>L145-B146</f>
+        <v>3569.95</v>
+      </c>
+      <c r="M146">
+        <v>59</v>
+      </c>
+      <c r="N146">
+        <f t="shared" si="141"/>
+        <v>9272.5299999999988</v>
+      </c>
+      <c r="O146">
+        <f t="shared" si="142"/>
+        <v>5272.5299999999988</v>
+      </c>
+      <c r="P146" s="25">
+        <f>O146-Ahorros!$E$4</f>
+        <v>272.52999999999884</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B147">
+        <v>22.83</v>
+      </c>
+      <c r="C147" t="s">
+        <v>212</v>
+      </c>
+      <c r="D147" t="s">
+        <v>82</v>
+      </c>
+      <c r="E147" t="s">
+        <v>22</v>
+      </c>
+      <c r="F147" t="s">
+        <v>18</v>
+      </c>
+      <c r="G147" t="s">
+        <v>84</v>
+      </c>
+      <c r="K147">
+        <v>5643.58</v>
+      </c>
+      <c r="L147">
+        <f>L146-B147</f>
+        <v>3547.12</v>
+      </c>
+      <c r="M147">
+        <v>59</v>
+      </c>
+      <c r="N147">
+        <f t="shared" si="141"/>
+        <v>9249.7000000000007</v>
+      </c>
+      <c r="O147">
+        <f t="shared" si="142"/>
+        <v>5249.7000000000007</v>
+      </c>
+      <c r="P147" s="25">
+        <f>O147-Ahorros!$E$4</f>
+        <v>249.70000000000073</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B148">
+        <v>6</v>
+      </c>
+      <c r="C148" t="s">
+        <v>128</v>
+      </c>
+      <c r="D148" t="s">
+        <v>128</v>
+      </c>
+      <c r="E148" t="s">
+        <v>22</v>
+      </c>
+      <c r="F148" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" t="s">
+        <v>84</v>
+      </c>
+      <c r="K148">
+        <v>5643.58</v>
+      </c>
+      <c r="L148">
+        <v>3547.12</v>
+      </c>
+      <c r="M148">
+        <f>M147-B148</f>
+        <v>53</v>
+      </c>
+      <c r="N148" s="39">
+        <f t="shared" ref="N148" si="143">SUM(K148:M148)</f>
+        <v>9243.7000000000007</v>
+      </c>
+      <c r="O148" s="39">
+        <f t="shared" ref="O148" si="144">N148-4000</f>
+        <v>5243.7000000000007</v>
+      </c>
+      <c r="P148" s="25">
+        <f>O148-Ahorros!$E$4</f>
+        <v>243.70000000000073</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>43590</v>
+      </c>
+      <c r="B149">
+        <v>85</v>
+      </c>
+      <c r="C149" t="s">
+        <v>93</v>
+      </c>
+      <c r="D149" t="s">
+        <v>93</v>
+      </c>
+      <c r="E149" t="s">
+        <v>22</v>
+      </c>
+      <c r="F149" t="s">
+        <v>131</v>
+      </c>
+      <c r="G149" t="s">
+        <v>93</v>
+      </c>
+      <c r="K149">
+        <f>K148-B149</f>
+        <v>5558.58</v>
+      </c>
+      <c r="L149">
+        <v>3547.12</v>
+      </c>
+      <c r="M149">
+        <v>53</v>
+      </c>
+      <c r="N149" s="39">
+        <f t="shared" ref="N149" si="145">SUM(K149:M149)</f>
+        <v>9158.7000000000007</v>
+      </c>
+      <c r="O149" s="39">
+        <f t="shared" ref="O149" si="146">N149-4000</f>
+        <v>5158.7000000000007</v>
+      </c>
+      <c r="P149" s="25">
+        <f>O149-Ahorros!$E$4</f>
+        <v>158.70000000000073</v>
       </c>
     </row>
   </sheetData>
@@ -7081,15 +7914,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Initial Data File Upload
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D682FD7C-B4B0-4CF7-9777-B92E1EAB9CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1E6BA-F754-4179-AC7C-43585843AC7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="252">
   <si>
     <t>Registro de transacciones en el periodo de Marzo de 2019</t>
   </si>
@@ -778,6 +778,45 @@
   </si>
   <si>
     <t>Rufles</t>
+  </si>
+  <si>
+    <t>Galletas</t>
+  </si>
+  <si>
+    <t>Ratón Logitech</t>
+  </si>
+  <si>
+    <t>Best Buy</t>
+  </si>
+  <si>
+    <t>Librero</t>
+  </si>
+  <si>
+    <t>Mobiliario</t>
+  </si>
+  <si>
+    <t>Mesa Auxiliar</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Azúcar</t>
+  </si>
+  <si>
+    <t>Sazonador Knorr</t>
+  </si>
+  <si>
+    <t>Palomitas Act II</t>
+  </si>
+  <si>
+    <t>Maruchan Camaron</t>
+  </si>
+  <si>
+    <t>Maruchan Res</t>
+  </si>
+  <si>
+    <t>Toalla de Cocina</t>
   </si>
 </sst>
 </file>
@@ -930,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -970,6 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1262,11 +1302,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V181"/>
+  <dimension ref="A1:V208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q181" sqref="Q181"/>
+      <pane ySplit="3" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,21 +1322,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -8393,11 +8433,11 @@
         <v>5</v>
       </c>
       <c r="N165" s="43">
-        <f t="shared" ref="N165:N181" si="162">SUM(K165:M165)</f>
+        <f t="shared" ref="N165:N183" si="162">SUM(K165:M165)</f>
         <v>8031.5400000000009</v>
       </c>
       <c r="O165" s="43">
-        <f t="shared" ref="O165:O181" si="163">N165-4000</f>
+        <f t="shared" ref="O165:O183" si="163">N165-4000</f>
         <v>4031.5400000000009</v>
       </c>
       <c r="P165" s="25">
@@ -9123,6 +9163,1222 @@
       <c r="P181" s="25">
         <f>O181-Ahorros!$E$4</f>
         <v>2029.4099999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B182">
+        <v>122.22</v>
+      </c>
+      <c r="C182" t="s">
+        <v>72</v>
+      </c>
+      <c r="D182" t="s">
+        <v>72</v>
+      </c>
+      <c r="E182" t="s">
+        <v>22</v>
+      </c>
+      <c r="F182" t="s">
+        <v>18</v>
+      </c>
+      <c r="G182" t="s">
+        <v>145</v>
+      </c>
+      <c r="K182">
+        <v>4856.18</v>
+      </c>
+      <c r="L182">
+        <f>L181-B182</f>
+        <v>6546.0099999999993</v>
+      </c>
+      <c r="M182">
+        <v>5</v>
+      </c>
+      <c r="N182">
+        <f t="shared" si="162"/>
+        <v>11407.189999999999</v>
+      </c>
+      <c r="O182">
+        <f t="shared" si="163"/>
+        <v>7407.1899999999987</v>
+      </c>
+      <c r="P182" s="25">
+        <f>O182-Ahorros!$E$4</f>
+        <v>1907.1899999999987</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B183">
+        <v>15</v>
+      </c>
+      <c r="C183" t="s">
+        <v>239</v>
+      </c>
+      <c r="D183" t="s">
+        <v>69</v>
+      </c>
+      <c r="E183" t="s">
+        <v>22</v>
+      </c>
+      <c r="F183" t="s">
+        <v>18</v>
+      </c>
+      <c r="G183" t="s">
+        <v>81</v>
+      </c>
+      <c r="K183">
+        <v>4856.18</v>
+      </c>
+      <c r="L183" s="46">
+        <f>L182-B183</f>
+        <v>6531.0099999999993</v>
+      </c>
+      <c r="M183">
+        <v>5</v>
+      </c>
+      <c r="N183">
+        <f t="shared" si="162"/>
+        <v>11392.189999999999</v>
+      </c>
+      <c r="O183">
+        <f t="shared" si="163"/>
+        <v>7392.1899999999987</v>
+      </c>
+      <c r="P183" s="25">
+        <f>O183-Ahorros!$E$4</f>
+        <v>1892.1899999999987</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B184">
+        <v>194</v>
+      </c>
+      <c r="C184" t="s">
+        <v>240</v>
+      </c>
+      <c r="D184" t="s">
+        <v>229</v>
+      </c>
+      <c r="E184" t="s">
+        <v>22</v>
+      </c>
+      <c r="F184" t="s">
+        <v>18</v>
+      </c>
+      <c r="G184" t="s">
+        <v>241</v>
+      </c>
+      <c r="K184">
+        <f>K183-B184</f>
+        <v>4662.18</v>
+      </c>
+      <c r="L184">
+        <v>6531.01</v>
+      </c>
+      <c r="M184">
+        <v>5</v>
+      </c>
+      <c r="N184" s="46">
+        <f t="shared" ref="N184" si="164">SUM(K184:M184)</f>
+        <v>11198.19</v>
+      </c>
+      <c r="O184" s="46">
+        <f t="shared" ref="O184" si="165">N184-4000</f>
+        <v>7198.1900000000005</v>
+      </c>
+      <c r="P184" s="25">
+        <f>O184-Ahorros!$E$4</f>
+        <v>1698.1900000000005</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B185">
+        <v>200</v>
+      </c>
+      <c r="C185" t="s">
+        <v>171</v>
+      </c>
+      <c r="D185" t="s">
+        <v>25</v>
+      </c>
+      <c r="E185" t="s">
+        <v>25</v>
+      </c>
+      <c r="F185" t="s">
+        <v>32</v>
+      </c>
+      <c r="G185" t="s">
+        <v>172</v>
+      </c>
+      <c r="K185">
+        <f>K184-B185</f>
+        <v>4462.18</v>
+      </c>
+      <c r="L185">
+        <v>6531.01</v>
+      </c>
+      <c r="M185">
+        <f>M184+B185</f>
+        <v>205</v>
+      </c>
+      <c r="N185" s="46">
+        <f t="shared" ref="N185" si="166">SUM(K185:M185)</f>
+        <v>11198.19</v>
+      </c>
+      <c r="O185" s="46">
+        <f t="shared" ref="O185" si="167">N185-4000</f>
+        <v>7198.1900000000005</v>
+      </c>
+      <c r="P185" s="25">
+        <f>O185-Ahorros!$E$4</f>
+        <v>1698.1900000000005</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B186">
+        <v>15</v>
+      </c>
+      <c r="C186" t="s">
+        <v>174</v>
+      </c>
+      <c r="D186" t="s">
+        <v>104</v>
+      </c>
+      <c r="E186" t="s">
+        <v>22</v>
+      </c>
+      <c r="F186" t="s">
+        <v>7</v>
+      </c>
+      <c r="G186" t="s">
+        <v>175</v>
+      </c>
+      <c r="K186">
+        <v>4462.18</v>
+      </c>
+      <c r="L186">
+        <v>6531.01</v>
+      </c>
+      <c r="M186">
+        <f>M185-B186</f>
+        <v>190</v>
+      </c>
+      <c r="N186" s="46">
+        <f t="shared" ref="N186" si="168">SUM(K186:M186)</f>
+        <v>11183.19</v>
+      </c>
+      <c r="O186" s="46">
+        <f t="shared" ref="O186" si="169">N186-4000</f>
+        <v>7183.1900000000005</v>
+      </c>
+      <c r="P186" s="25">
+        <f>O186-Ahorros!$E$4</f>
+        <v>1683.1900000000005</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B187">
+        <v>459</v>
+      </c>
+      <c r="C187" t="s">
+        <v>242</v>
+      </c>
+      <c r="D187" t="s">
+        <v>243</v>
+      </c>
+      <c r="E187" t="s">
+        <v>22</v>
+      </c>
+      <c r="F187" t="s">
+        <v>18</v>
+      </c>
+      <c r="G187" t="s">
+        <v>84</v>
+      </c>
+      <c r="K187">
+        <v>4462.18</v>
+      </c>
+      <c r="L187">
+        <f>L186-B187</f>
+        <v>6072.01</v>
+      </c>
+      <c r="M187">
+        <v>190</v>
+      </c>
+      <c r="N187" s="46">
+        <f t="shared" ref="N187:N188" si="170">SUM(K187:M187)</f>
+        <v>10724.19</v>
+      </c>
+      <c r="O187" s="46">
+        <f t="shared" ref="O187:O188" si="171">N187-4000</f>
+        <v>6724.1900000000005</v>
+      </c>
+      <c r="P187" s="25">
+        <f>O187-Ahorros!$E$4</f>
+        <v>1224.1900000000005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B188">
+        <v>239</v>
+      </c>
+      <c r="C188" t="s">
+        <v>244</v>
+      </c>
+      <c r="D188" t="s">
+        <v>243</v>
+      </c>
+      <c r="E188" t="s">
+        <v>22</v>
+      </c>
+      <c r="F188" t="s">
+        <v>18</v>
+      </c>
+      <c r="G188" t="s">
+        <v>84</v>
+      </c>
+      <c r="K188">
+        <v>4462.18</v>
+      </c>
+      <c r="L188" s="46">
+        <f>L187-B188</f>
+        <v>5833.01</v>
+      </c>
+      <c r="M188">
+        <v>190</v>
+      </c>
+      <c r="N188">
+        <f t="shared" si="170"/>
+        <v>10485.19</v>
+      </c>
+      <c r="O188">
+        <f t="shared" si="171"/>
+        <v>6485.1900000000005</v>
+      </c>
+      <c r="P188" s="25">
+        <f>O188-Ahorros!$E$4</f>
+        <v>985.19000000000051</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B189">
+        <v>15</v>
+      </c>
+      <c r="C189" t="s">
+        <v>231</v>
+      </c>
+      <c r="D189" t="s">
+        <v>82</v>
+      </c>
+      <c r="E189" t="s">
+        <v>22</v>
+      </c>
+      <c r="F189" t="s">
+        <v>18</v>
+      </c>
+      <c r="G189" t="s">
+        <v>84</v>
+      </c>
+      <c r="K189">
+        <v>4462.18</v>
+      </c>
+      <c r="L189" s="46">
+        <f>L188-B189</f>
+        <v>5818.01</v>
+      </c>
+      <c r="M189">
+        <v>190</v>
+      </c>
+      <c r="N189" s="46">
+        <f t="shared" ref="N189:N204" si="172">SUM(K189:M189)</f>
+        <v>10470.19</v>
+      </c>
+      <c r="O189" s="46">
+        <f t="shared" ref="O189:O204" si="173">N189-4000</f>
+        <v>6470.1900000000005</v>
+      </c>
+      <c r="P189" s="25">
+        <f>O189-Ahorros!$E$4</f>
+        <v>970.19000000000051</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B190">
+        <v>12.95</v>
+      </c>
+      <c r="C190" t="s">
+        <v>245</v>
+      </c>
+      <c r="D190" t="s">
+        <v>82</v>
+      </c>
+      <c r="E190" t="s">
+        <v>22</v>
+      </c>
+      <c r="F190" t="s">
+        <v>18</v>
+      </c>
+      <c r="G190" t="s">
+        <v>84</v>
+      </c>
+      <c r="K190">
+        <v>4462.18</v>
+      </c>
+      <c r="L190">
+        <f>L189-B190</f>
+        <v>5805.06</v>
+      </c>
+      <c r="M190">
+        <v>190</v>
+      </c>
+      <c r="N190">
+        <f t="shared" si="172"/>
+        <v>10457.240000000002</v>
+      </c>
+      <c r="O190">
+        <f t="shared" si="173"/>
+        <v>6457.2400000000016</v>
+      </c>
+      <c r="P190" s="25">
+        <f>O190-Ahorros!$E$4</f>
+        <v>957.2400000000016</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B191">
+        <v>19.55</v>
+      </c>
+      <c r="C191" t="s">
+        <v>146</v>
+      </c>
+      <c r="D191" t="s">
+        <v>82</v>
+      </c>
+      <c r="E191" t="s">
+        <v>22</v>
+      </c>
+      <c r="F191" t="s">
+        <v>18</v>
+      </c>
+      <c r="G191" t="s">
+        <v>84</v>
+      </c>
+      <c r="K191">
+        <v>4462.18</v>
+      </c>
+      <c r="L191" s="46">
+        <f>L190-B191</f>
+        <v>5785.51</v>
+      </c>
+      <c r="M191">
+        <v>190</v>
+      </c>
+      <c r="N191">
+        <f t="shared" si="172"/>
+        <v>10437.69</v>
+      </c>
+      <c r="O191">
+        <f t="shared" si="173"/>
+        <v>6437.6900000000005</v>
+      </c>
+      <c r="P191" s="25">
+        <f>O191-Ahorros!$E$4</f>
+        <v>937.69000000000051</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B192">
+        <v>26</v>
+      </c>
+      <c r="C192" t="s">
+        <v>246</v>
+      </c>
+      <c r="D192" t="s">
+        <v>82</v>
+      </c>
+      <c r="E192" t="s">
+        <v>22</v>
+      </c>
+      <c r="F192" t="s">
+        <v>18</v>
+      </c>
+      <c r="G192" t="s">
+        <v>84</v>
+      </c>
+      <c r="K192">
+        <v>4462.18</v>
+      </c>
+      <c r="L192" s="46">
+        <f>L191-B192</f>
+        <v>5759.51</v>
+      </c>
+      <c r="M192">
+        <v>190</v>
+      </c>
+      <c r="N192">
+        <f t="shared" si="172"/>
+        <v>10411.69</v>
+      </c>
+      <c r="O192">
+        <f t="shared" si="173"/>
+        <v>6411.6900000000005</v>
+      </c>
+      <c r="P192" s="25">
+        <f>O192-Ahorros!$E$4</f>
+        <v>911.69000000000051</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B193">
+        <v>43</v>
+      </c>
+      <c r="C193" t="s">
+        <v>126</v>
+      </c>
+      <c r="D193" t="s">
+        <v>82</v>
+      </c>
+      <c r="E193" t="s">
+        <v>22</v>
+      </c>
+      <c r="F193" t="s">
+        <v>18</v>
+      </c>
+      <c r="G193" t="s">
+        <v>84</v>
+      </c>
+      <c r="K193">
+        <v>4462.18</v>
+      </c>
+      <c r="L193" s="46">
+        <f>L192-B193</f>
+        <v>5716.51</v>
+      </c>
+      <c r="M193">
+        <v>190</v>
+      </c>
+      <c r="N193">
+        <f t="shared" si="172"/>
+        <v>10368.69</v>
+      </c>
+      <c r="O193">
+        <f t="shared" si="173"/>
+        <v>6368.6900000000005</v>
+      </c>
+      <c r="P193" s="25">
+        <f>O193-Ahorros!$E$4</f>
+        <v>868.69000000000051</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B194">
+        <v>26.9</v>
+      </c>
+      <c r="C194" t="s">
+        <v>147</v>
+      </c>
+      <c r="D194" t="s">
+        <v>82</v>
+      </c>
+      <c r="E194" t="s">
+        <v>22</v>
+      </c>
+      <c r="F194" t="s">
+        <v>18</v>
+      </c>
+      <c r="G194" t="s">
+        <v>84</v>
+      </c>
+      <c r="K194">
+        <v>4462.18</v>
+      </c>
+      <c r="L194" s="46">
+        <f>L193-B194</f>
+        <v>5689.6100000000006</v>
+      </c>
+      <c r="M194">
+        <v>190</v>
+      </c>
+      <c r="N194">
+        <f t="shared" si="172"/>
+        <v>10341.790000000001</v>
+      </c>
+      <c r="O194">
+        <f t="shared" si="173"/>
+        <v>6341.7900000000009</v>
+      </c>
+      <c r="P194" s="25">
+        <f>O194-Ahorros!$E$4</f>
+        <v>841.79000000000087</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B195">
+        <v>15.65</v>
+      </c>
+      <c r="C195" t="s">
+        <v>247</v>
+      </c>
+      <c r="D195" t="s">
+        <v>82</v>
+      </c>
+      <c r="E195" t="s">
+        <v>22</v>
+      </c>
+      <c r="F195" t="s">
+        <v>18</v>
+      </c>
+      <c r="G195" t="s">
+        <v>84</v>
+      </c>
+      <c r="K195">
+        <v>4462.18</v>
+      </c>
+      <c r="L195" s="46">
+        <f>L194-B195</f>
+        <v>5673.9600000000009</v>
+      </c>
+      <c r="M195">
+        <v>190</v>
+      </c>
+      <c r="N195">
+        <f t="shared" si="172"/>
+        <v>10326.140000000001</v>
+      </c>
+      <c r="O195">
+        <f t="shared" si="173"/>
+        <v>6326.1400000000012</v>
+      </c>
+      <c r="P195" s="25">
+        <f>O195-Ahorros!$E$4</f>
+        <v>826.14000000000124</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B196">
+        <v>56.6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>83</v>
+      </c>
+      <c r="D196" t="s">
+        <v>82</v>
+      </c>
+      <c r="E196" t="s">
+        <v>22</v>
+      </c>
+      <c r="F196" t="s">
+        <v>18</v>
+      </c>
+      <c r="G196" t="s">
+        <v>84</v>
+      </c>
+      <c r="K196">
+        <v>4462.18</v>
+      </c>
+      <c r="L196" s="46">
+        <f>L195-B196</f>
+        <v>5617.3600000000006</v>
+      </c>
+      <c r="M196">
+        <v>190</v>
+      </c>
+      <c r="N196">
+        <f t="shared" si="172"/>
+        <v>10269.540000000001</v>
+      </c>
+      <c r="O196">
+        <f t="shared" si="173"/>
+        <v>6269.5400000000009</v>
+      </c>
+      <c r="P196" s="25">
+        <f>O196-Ahorros!$E$4</f>
+        <v>769.54000000000087</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B197">
+        <v>13.5</v>
+      </c>
+      <c r="C197" t="s">
+        <v>182</v>
+      </c>
+      <c r="D197" t="s">
+        <v>82</v>
+      </c>
+      <c r="E197" t="s">
+        <v>22</v>
+      </c>
+      <c r="F197" t="s">
+        <v>18</v>
+      </c>
+      <c r="G197" t="s">
+        <v>84</v>
+      </c>
+      <c r="K197">
+        <v>4462.18</v>
+      </c>
+      <c r="L197" s="46">
+        <f>L196-B197</f>
+        <v>5603.8600000000006</v>
+      </c>
+      <c r="M197">
+        <v>190</v>
+      </c>
+      <c r="N197">
+        <f t="shared" si="172"/>
+        <v>10256.040000000001</v>
+      </c>
+      <c r="O197">
+        <f t="shared" si="173"/>
+        <v>6256.0400000000009</v>
+      </c>
+      <c r="P197" s="25">
+        <f>O197-Ahorros!$E$4</f>
+        <v>756.04000000000087</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B198">
+        <v>25.5</v>
+      </c>
+      <c r="C198" t="s">
+        <v>152</v>
+      </c>
+      <c r="D198" t="s">
+        <v>82</v>
+      </c>
+      <c r="E198" t="s">
+        <v>22</v>
+      </c>
+      <c r="F198" t="s">
+        <v>18</v>
+      </c>
+      <c r="G198" t="s">
+        <v>84</v>
+      </c>
+      <c r="K198">
+        <v>4462.18</v>
+      </c>
+      <c r="L198" s="46">
+        <f>L197-B198</f>
+        <v>5578.3600000000006</v>
+      </c>
+      <c r="M198">
+        <v>190</v>
+      </c>
+      <c r="N198">
+        <f t="shared" si="172"/>
+        <v>10230.540000000001</v>
+      </c>
+      <c r="O198">
+        <f t="shared" si="173"/>
+        <v>6230.5400000000009</v>
+      </c>
+      <c r="P198" s="25">
+        <f>O198-Ahorros!$E$4</f>
+        <v>730.54000000000087</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B199">
+        <v>22.25</v>
+      </c>
+      <c r="C199" t="s">
+        <v>153</v>
+      </c>
+      <c r="D199" t="s">
+        <v>82</v>
+      </c>
+      <c r="E199" t="s">
+        <v>22</v>
+      </c>
+      <c r="F199" t="s">
+        <v>18</v>
+      </c>
+      <c r="G199" t="s">
+        <v>84</v>
+      </c>
+      <c r="K199">
+        <v>4462.18</v>
+      </c>
+      <c r="L199" s="46">
+        <f>L198-B199</f>
+        <v>5556.1100000000006</v>
+      </c>
+      <c r="M199">
+        <v>190</v>
+      </c>
+      <c r="N199">
+        <f t="shared" si="172"/>
+        <v>10208.290000000001</v>
+      </c>
+      <c r="O199">
+        <f t="shared" si="173"/>
+        <v>6208.2900000000009</v>
+      </c>
+      <c r="P199" s="25">
+        <f>O199-Ahorros!$E$4</f>
+        <v>708.29000000000087</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B200">
+        <v>10.6</v>
+      </c>
+      <c r="C200" t="s">
+        <v>248</v>
+      </c>
+      <c r="D200" t="s">
+        <v>82</v>
+      </c>
+      <c r="E200" t="s">
+        <v>22</v>
+      </c>
+      <c r="F200" t="s">
+        <v>18</v>
+      </c>
+      <c r="G200" t="s">
+        <v>84</v>
+      </c>
+      <c r="K200">
+        <v>4462.18</v>
+      </c>
+      <c r="L200" s="46">
+        <f>L199-B200</f>
+        <v>5545.51</v>
+      </c>
+      <c r="M200">
+        <v>190</v>
+      </c>
+      <c r="N200">
+        <f t="shared" si="172"/>
+        <v>10197.69</v>
+      </c>
+      <c r="O200">
+        <f t="shared" si="173"/>
+        <v>6197.6900000000005</v>
+      </c>
+      <c r="P200" s="25">
+        <f>O200-Ahorros!$E$4</f>
+        <v>697.69000000000051</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B201">
+        <v>37.25</v>
+      </c>
+      <c r="C201" t="s">
+        <v>87</v>
+      </c>
+      <c r="D201" t="s">
+        <v>82</v>
+      </c>
+      <c r="E201" t="s">
+        <v>22</v>
+      </c>
+      <c r="F201" t="s">
+        <v>18</v>
+      </c>
+      <c r="G201" t="s">
+        <v>84</v>
+      </c>
+      <c r="K201">
+        <v>4462.18</v>
+      </c>
+      <c r="L201" s="46">
+        <f>L200-B201</f>
+        <v>5508.26</v>
+      </c>
+      <c r="M201">
+        <v>190</v>
+      </c>
+      <c r="N201">
+        <f t="shared" si="172"/>
+        <v>10160.44</v>
+      </c>
+      <c r="O201">
+        <f t="shared" si="173"/>
+        <v>6160.4400000000005</v>
+      </c>
+      <c r="P201" s="25">
+        <f>O201-Ahorros!$E$4</f>
+        <v>660.44000000000051</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B202">
+        <v>9.5</v>
+      </c>
+      <c r="C202" t="s">
+        <v>249</v>
+      </c>
+      <c r="D202" t="s">
+        <v>82</v>
+      </c>
+      <c r="E202" t="s">
+        <v>22</v>
+      </c>
+      <c r="F202" t="s">
+        <v>18</v>
+      </c>
+      <c r="G202" t="s">
+        <v>84</v>
+      </c>
+      <c r="K202">
+        <v>4462.18</v>
+      </c>
+      <c r="L202" s="46">
+        <f>L201-B202</f>
+        <v>5498.76</v>
+      </c>
+      <c r="M202">
+        <v>190</v>
+      </c>
+      <c r="N202">
+        <f t="shared" si="172"/>
+        <v>10150.94</v>
+      </c>
+      <c r="O202">
+        <f t="shared" si="173"/>
+        <v>6150.9400000000005</v>
+      </c>
+      <c r="P202" s="25">
+        <f>O202-Ahorros!$E$4</f>
+        <v>650.94000000000051</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B203">
+        <v>9.5</v>
+      </c>
+      <c r="C203" t="s">
+        <v>250</v>
+      </c>
+      <c r="D203" t="s">
+        <v>82</v>
+      </c>
+      <c r="E203" t="s">
+        <v>22</v>
+      </c>
+      <c r="F203" t="s">
+        <v>18</v>
+      </c>
+      <c r="G203" t="s">
+        <v>84</v>
+      </c>
+      <c r="K203">
+        <v>4462.18</v>
+      </c>
+      <c r="L203" s="46">
+        <f>L202-B203</f>
+        <v>5489.26</v>
+      </c>
+      <c r="M203">
+        <v>190</v>
+      </c>
+      <c r="N203">
+        <f t="shared" si="172"/>
+        <v>10141.44</v>
+      </c>
+      <c r="O203">
+        <f t="shared" si="173"/>
+        <v>6141.4400000000005</v>
+      </c>
+      <c r="P203" s="25">
+        <f>O203-Ahorros!$E$4</f>
+        <v>641.44000000000051</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B204">
+        <v>11.5</v>
+      </c>
+      <c r="C204" t="s">
+        <v>251</v>
+      </c>
+      <c r="D204" t="s">
+        <v>220</v>
+      </c>
+      <c r="E204" t="s">
+        <v>22</v>
+      </c>
+      <c r="F204" t="s">
+        <v>18</v>
+      </c>
+      <c r="G204" t="s">
+        <v>84</v>
+      </c>
+      <c r="K204">
+        <v>4462.18</v>
+      </c>
+      <c r="L204" s="46">
+        <f>L203-B204</f>
+        <v>5477.76</v>
+      </c>
+      <c r="M204">
+        <v>190</v>
+      </c>
+      <c r="N204">
+        <f t="shared" si="172"/>
+        <v>10129.94</v>
+      </c>
+      <c r="O204">
+        <f t="shared" si="173"/>
+        <v>6129.9400000000005</v>
+      </c>
+      <c r="P204" s="25">
+        <f>O204-Ahorros!$E$4</f>
+        <v>629.94000000000051</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B205">
+        <v>225</v>
+      </c>
+      <c r="C205" t="s">
+        <v>157</v>
+      </c>
+      <c r="D205" t="s">
+        <v>48</v>
+      </c>
+      <c r="E205" t="s">
+        <v>22</v>
+      </c>
+      <c r="F205" t="s">
+        <v>32</v>
+      </c>
+      <c r="G205" t="s">
+        <v>49</v>
+      </c>
+      <c r="K205">
+        <f>K204-B205</f>
+        <v>4237.18</v>
+      </c>
+      <c r="L205">
+        <v>5477.76</v>
+      </c>
+      <c r="M205">
+        <v>190</v>
+      </c>
+      <c r="N205" s="46">
+        <f t="shared" ref="N205" si="174">SUM(K205:M205)</f>
+        <v>9904.94</v>
+      </c>
+      <c r="O205" s="46">
+        <f t="shared" ref="O205" si="175">N205-4000</f>
+        <v>5904.9400000000005</v>
+      </c>
+      <c r="P205" s="25">
+        <f>O205-Ahorros!$E$4</f>
+        <v>404.94000000000051</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B206">
+        <v>15</v>
+      </c>
+      <c r="C206" t="s">
+        <v>176</v>
+      </c>
+      <c r="D206" t="s">
+        <v>128</v>
+      </c>
+      <c r="E206" t="s">
+        <v>22</v>
+      </c>
+      <c r="F206" t="s">
+        <v>7</v>
+      </c>
+      <c r="G206" t="s">
+        <v>84</v>
+      </c>
+      <c r="K206">
+        <v>4237.18</v>
+      </c>
+      <c r="L206">
+        <v>5477.76</v>
+      </c>
+      <c r="M206">
+        <f>M205-B206</f>
+        <v>175</v>
+      </c>
+      <c r="N206" s="46">
+        <f t="shared" ref="N206:N208" si="176">SUM(K206:M206)</f>
+        <v>9889.94</v>
+      </c>
+      <c r="O206" s="46">
+        <f t="shared" ref="O206:O208" si="177">N206-4000</f>
+        <v>5889.9400000000005</v>
+      </c>
+      <c r="P206" s="25">
+        <f>O206-Ahorros!$E$4</f>
+        <v>389.94000000000051</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B207">
+        <v>38</v>
+      </c>
+      <c r="C207" t="s">
+        <v>99</v>
+      </c>
+      <c r="D207" t="s">
+        <v>82</v>
+      </c>
+      <c r="E207" t="s">
+        <v>22</v>
+      </c>
+      <c r="F207" t="s">
+        <v>7</v>
+      </c>
+      <c r="G207" t="s">
+        <v>81</v>
+      </c>
+      <c r="K207">
+        <v>4237.18</v>
+      </c>
+      <c r="L207">
+        <v>5477.76</v>
+      </c>
+      <c r="M207">
+        <f>M206-B207</f>
+        <v>137</v>
+      </c>
+      <c r="N207">
+        <f t="shared" si="176"/>
+        <v>9851.94</v>
+      </c>
+      <c r="O207">
+        <f t="shared" si="177"/>
+        <v>5851.9400000000005</v>
+      </c>
+      <c r="P207" s="25">
+        <f>O207-Ahorros!$E$4</f>
+        <v>351.94000000000051</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B208">
+        <v>10</v>
+      </c>
+      <c r="C208" t="s">
+        <v>177</v>
+      </c>
+      <c r="D208" t="s">
+        <v>43</v>
+      </c>
+      <c r="E208" t="s">
+        <v>22</v>
+      </c>
+      <c r="F208" t="s">
+        <v>7</v>
+      </c>
+      <c r="G208" t="s">
+        <v>44</v>
+      </c>
+      <c r="K208">
+        <v>4237.18</v>
+      </c>
+      <c r="L208">
+        <v>5477.76</v>
+      </c>
+      <c r="M208">
+        <f>M207-B208</f>
+        <v>127</v>
+      </c>
+      <c r="N208">
+        <f t="shared" si="176"/>
+        <v>9841.94</v>
+      </c>
+      <c r="O208">
+        <f t="shared" si="177"/>
+        <v>5841.9400000000005</v>
+      </c>
+      <c r="P208" s="25">
+        <f>O208-Ahorros!$E$4</f>
+        <v>341.94000000000051</v>
       </c>
     </row>
   </sheetData>
@@ -9439,7 +10695,7 @@
   <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9449,15 +10705,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9518,6 +10774,12 @@
       </c>
       <c r="B7">
         <v>500</v>
+      </c>
+      <c r="H7">
+        <v>5000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>43603</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created CSV test Files, Basic Script for calculations created
</commit_message>
<xml_diff>
--- a/data/initial_data.xlsx
+++ b/data/initial_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FCAB93-B7C0-49A0-9ECD-428EC38157A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46AED5E-AFAC-410E-BB21-0F657AB5DB9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1398,8 +1398,8 @@
   <dimension ref="A1:V243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K244" sqref="K244"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11040,7 +11040,7 @@
         <v>4103.18</v>
       </c>
       <c r="L221">
-        <f>L220-B221</f>
+        <f t="shared" ref="L221:L240" si="194">L220-B221</f>
         <v>4915.4100000000008</v>
       </c>
       <c r="M221">
@@ -11085,7 +11085,7 @@
         <v>4103.18</v>
       </c>
       <c r="L222" s="49">
-        <f>L221-B222</f>
+        <f t="shared" si="194"/>
         <v>4892.8300000000008</v>
       </c>
       <c r="M222">
@@ -11130,7 +11130,7 @@
         <v>4103.18</v>
       </c>
       <c r="L223" s="49">
-        <f>L222-B223</f>
+        <f t="shared" si="194"/>
         <v>4881.6800000000012</v>
       </c>
       <c r="M223">
@@ -11175,7 +11175,7 @@
         <v>4103.18</v>
       </c>
       <c r="L224" s="49">
-        <f>L223-B224</f>
+        <f t="shared" si="194"/>
         <v>4868.7800000000016</v>
       </c>
       <c r="M224">
@@ -11220,7 +11220,7 @@
         <v>4103.18</v>
       </c>
       <c r="L225" s="49">
-        <f>L224-B225</f>
+        <f t="shared" si="194"/>
         <v>4847.7800000000016</v>
       </c>
       <c r="M225">
@@ -11265,7 +11265,7 @@
         <v>4103.18</v>
       </c>
       <c r="L226" s="49">
-        <f>L225-B226</f>
+        <f t="shared" si="194"/>
         <v>4829.6800000000012</v>
       </c>
       <c r="M226">
@@ -11310,7 +11310,7 @@
         <v>4103.18</v>
       </c>
       <c r="L227" s="49">
-        <f>L226-B227</f>
+        <f t="shared" si="194"/>
         <v>4785.6800000000012</v>
       </c>
       <c r="M227">
@@ -11355,7 +11355,7 @@
         <v>4103.18</v>
       </c>
       <c r="L228" s="49">
-        <f>L227-B228</f>
+        <f t="shared" si="194"/>
         <v>4753.1100000000015</v>
       </c>
       <c r="M228">
@@ -11400,7 +11400,7 @@
         <v>4103.18</v>
       </c>
       <c r="L229" s="49">
-        <f>L228-B229</f>
+        <f t="shared" si="194"/>
         <v>4716.8600000000015</v>
       </c>
       <c r="M229">
@@ -11445,7 +11445,7 @@
         <v>4103.18</v>
       </c>
       <c r="L230" s="49">
-        <f>L229-B230</f>
+        <f t="shared" si="194"/>
         <v>4689.2600000000011</v>
       </c>
       <c r="M230">
@@ -11490,7 +11490,7 @@
         <v>4103.18</v>
       </c>
       <c r="L231" s="49">
-        <f>L230-B231</f>
+        <f t="shared" si="194"/>
         <v>4673.6800000000012</v>
       </c>
       <c r="M231">
@@ -11535,7 +11535,7 @@
         <v>4103.18</v>
       </c>
       <c r="L232" s="49">
-        <f>L231-B232</f>
+        <f t="shared" si="194"/>
         <v>4651.6800000000012</v>
       </c>
       <c r="M232">
@@ -11580,7 +11580,7 @@
         <v>4103.18</v>
       </c>
       <c r="L233" s="49">
-        <f>L232-B233</f>
+        <f t="shared" si="194"/>
         <v>4642.630000000001</v>
       </c>
       <c r="M233">
@@ -11625,7 +11625,7 @@
         <v>4103.18</v>
       </c>
       <c r="L234" s="49">
-        <f>L233-B234</f>
+        <f t="shared" si="194"/>
         <v>4638.3300000000008</v>
       </c>
       <c r="M234">
@@ -11670,7 +11670,7 @@
         <v>4103.18</v>
       </c>
       <c r="L235" s="49">
-        <f>L234-B235</f>
+        <f t="shared" si="194"/>
         <v>4627.3300000000008</v>
       </c>
       <c r="M235">
@@ -11715,7 +11715,7 @@
         <v>4103.18</v>
       </c>
       <c r="L236" s="49">
-        <f>L235-B236</f>
+        <f t="shared" si="194"/>
         <v>4611.8300000000008</v>
       </c>
       <c r="M236">
@@ -11760,7 +11760,7 @@
         <v>4103.18</v>
       </c>
       <c r="L237" s="49">
-        <f>L236-B237</f>
+        <f t="shared" si="194"/>
         <v>4526.8300000000008</v>
       </c>
       <c r="M237">
@@ -11805,7 +11805,7 @@
         <v>4103.18</v>
       </c>
       <c r="L238" s="49">
-        <f>L237-B238</f>
+        <f t="shared" si="194"/>
         <v>4224.8300000000008</v>
       </c>
       <c r="M238">
@@ -11850,7 +11850,7 @@
         <v>4103.18</v>
       </c>
       <c r="L239" s="49">
-        <f>L238-B239</f>
+        <f t="shared" si="194"/>
         <v>4199.8300000000008</v>
       </c>
       <c r="M239">
@@ -11895,7 +11895,7 @@
         <v>4103.18</v>
       </c>
       <c r="L240" s="49">
-        <f>L239-B240</f>
+        <f t="shared" si="194"/>
         <v>499.83000000000084</v>
       </c>
       <c r="M240">
@@ -11947,11 +11947,11 @@
         <v>107</v>
       </c>
       <c r="N241" s="49">
-        <f t="shared" ref="N241" si="194">SUM(K241:M241)</f>
+        <f t="shared" ref="N241" si="195">SUM(K241:M241)</f>
         <v>4661.01</v>
       </c>
       <c r="O241" s="49">
-        <f t="shared" ref="O241" si="195">N241-4000</f>
+        <f t="shared" ref="O241" si="196">N241-4000</f>
         <v>661.01000000000022</v>
       </c>
       <c r="P241" s="25">
@@ -11992,11 +11992,11 @@
         <v>39</v>
       </c>
       <c r="N242" s="49">
-        <f t="shared" ref="N242" si="196">SUM(K242:M242)</f>
+        <f t="shared" ref="N242" si="197">SUM(K242:M242)</f>
         <v>4593.01</v>
       </c>
       <c r="O242" s="49">
-        <f t="shared" ref="O242" si="197">N242-4000</f>
+        <f t="shared" ref="O242" si="198">N242-4000</f>
         <v>593.01000000000022</v>
       </c>
       <c r="P242" s="25">
@@ -12037,11 +12037,11 @@
         <v>29</v>
       </c>
       <c r="N243" s="49">
-        <f t="shared" ref="N243" si="198">SUM(K243:M243)</f>
+        <f t="shared" ref="N243" si="199">SUM(K243:M243)</f>
         <v>4583.01</v>
       </c>
       <c r="O243" s="49">
-        <f t="shared" ref="O243" si="199">N243-4000</f>
+        <f t="shared" ref="O243" si="200">N243-4000</f>
         <v>583.01000000000022</v>
       </c>
       <c r="P243" s="25">

</xml_diff>